<commit_message>
Perfil - Ideas a Defender
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACIÓN/1.2 Cronograma/GN1_Cronograma_V1.xlsx
+++ b/PREGAME/1. ELICITACIÓN/1.2 Cronograma/GN1_Cronograma_V1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D6AA4C-918D-412D-B6BE-5DAEC6F56A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F7262F-AFCC-4146-A8BC-A6C589F73464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1222,8 +1222,8 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1430,7 +1430,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F12" s="8">
         <v>45996</v>
@@ -1439,7 +1439,7 @@
         <v>46002</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,35 +1869,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2197,27 +2168,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C9377B5-33A9-4C3D-9A88-86A3E387B080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D80D6D39-DBD9-4440-B62F-A6A353ABBEAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828CA8E1-44D4-4665-B868-FBF7A439CAC3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2236,4 +2216,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D80D6D39-DBD9-4440-B62F-A6A353ABBEAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C9377B5-33A9-4C3D-9A88-86A3E387B080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>